<commit_message>
Fix XML rappel with caution
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_virements_xlsx/état_des_virements_10_2022.xlsx
+++ b/download/generated situation/état_des_virements_xlsx/état_des_virements_10_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -417,182 +417,77 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>MOHAMED BADRANE</v>
+        <v>NASIRI HASNAA</v>
       </c>
       <c r="B2" t="str">
-        <v>I83603</v>
+        <v/>
       </c>
       <c r="C2" t="str">
-        <v>225400000805987601012173</v>
+        <v>546576878798989898090090</v>
       </c>
       <c r="D2" t="str">
-        <v>KHOURIBGA</v>
+        <v/>
       </c>
       <c r="E2" t="str">
-        <v>CA</v>
+        <v>CIH</v>
       </c>
       <c r="F2" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="G2" t="str">
-        <v>605/KHOURIBGA NAHDA</v>
+        <v>901/CASABLANCA</v>
       </c>
       <c r="H2" t="str">
         <v>mensuelle</v>
       </c>
       <c r="I2">
-        <v>7500</v>
+        <v>8000.01</v>
       </c>
       <c r="J2">
-        <v>375</v>
+        <v>800.01</v>
       </c>
       <c r="K2">
-        <v>7125</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>ZERNAKH ABDELLAH</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B3" t="str">
-        <v>IB19558</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C3" t="str">
-        <v>145101211406073828000084</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D3" t="str">
-        <v>MARRAKECH BENI MELLAL</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E3" t="str">
-        <v>BP</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F3" t="str">
-        <v>Point de vente</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="G3" t="str">
-        <v>052/FKIH BEN SALEH</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H3" t="str">
-        <v>mensuelle</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="I3">
-        <v>11000</v>
+        <v>8000.01</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>800.01</v>
       </c>
       <c r="K3">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>NOUBAIL MOUNTASSIR</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Q251990</v>
-      </c>
-      <c r="C4" t="str">
-        <v>007400000313200019604463</v>
-      </c>
-      <c r="D4" t="str">
-        <v>KHOURIBGA ZELLAKA</v>
-      </c>
-      <c r="E4" t="str">
-        <v>AWB</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G4" t="str">
-        <v>905/TADLA OUARDIGHA ZAYANE</v>
-      </c>
-      <c r="H4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I4">
-        <v>6750</v>
-      </c>
-      <c r="J4">
-        <v>675</v>
-      </c>
-      <c r="K4">
-        <v>6075</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>NOUBAIL MOHAMMED</v>
-      </c>
-      <c r="B5" t="str">
-        <v>IR801997</v>
-      </c>
-      <c r="C5" t="str">
-        <v>007400000313200019604463</v>
-      </c>
-      <c r="D5" t="str">
-        <v>KHOURIBGA ZELLAKA</v>
-      </c>
-      <c r="E5" t="str">
-        <v>AWB</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="G5" t="str">
-        <v>905/TADLA OUARDIGHA ZAYANE</v>
-      </c>
-      <c r="H5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="I5">
-        <v>6750</v>
-      </c>
-      <c r="J5">
-        <v>675</v>
-      </c>
-      <c r="K5">
-        <v>6075</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H6" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I6">
-        <v>32000</v>
-      </c>
-      <c r="J6">
-        <v>1725</v>
-      </c>
-      <c r="K6">
-        <v>30275</v>
+        <v>7200</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>